<commit_message>
Feat. make dummy datas
</commit_message>
<xml_diff>
--- a/dummy-03.xlsx
+++ b/dummy-03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minsukim/Desktop/devminsu/GITHUB/Read-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1132B6C3-60DD-3B48-A9FD-B46D30079385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61436B78-E2CE-F040-9D44-00493E3E421B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="14400" windowHeight="17380" activeTab="1" xr2:uid="{04869455-A2F6-0641-A8AA-6D8E25974CAD}"/>
   </bookViews>
@@ -2137,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D9FAFE-43BB-BC42-BA9D-120B41B79FDE}">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>